<commit_message>
board order ready, BOM updated with purchasable parts
</commit_message>
<xml_diff>
--- a/powerwatch/hardware/plugwatch_E/board/plugwatch_bom.xlsx
+++ b/powerwatch/hardware/plugwatch_E/board/plugwatch_bom.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="plugwatch" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="plugwatch_bom" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="313">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">SPICEPREFIX</t>
   </si>
   <si>
-    <t xml:space="preserve">DIODE_SCHOTTKYSOD323</t>
+    <t xml:space="preserve">DIODE_ZENERSOT323</t>
   </si>
   <si>
     <t xml:space="preserve">SOD323</t>
@@ -67,21 +67,6 @@
     <t xml:space="preserve">D1,D2,D3,D4</t>
   </si>
   <si>
-    <t xml:space="preserve">CUS10S30H3FCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toshiba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CUS10S30,H3F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIODE_ZENERSOT323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D5,D6,D7,D8</t>
-  </si>
-  <si>
     <t xml:space="preserve">DIODE ZENER 3.3V 200MW SOD323F</t>
   </si>
   <si>
@@ -142,12 +127,15 @@
     <t xml:space="preserve">SPH0465</t>
   </si>
   <si>
-    <t xml:space="preserve">U14</t>
+    <t xml:space="preserve">U15</t>
   </si>
   <si>
     <t xml:space="preserve">An I2S microphone down to 20hz</t>
   </si>
   <si>
+    <t xml:space="preserve">423-1405-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">Knowles</t>
   </si>
   <si>
@@ -196,7 +184,7 @@
     <t xml:space="preserve">GRM155C80J824KE15D</t>
   </si>
   <si>
-    <t xml:space="preserve">1.5k</t>
+    <t xml:space="preserve">100k</t>
   </si>
   <si>
     <t xml:space="preserve">RESISTOR0402_RES</t>
@@ -205,285 +193,255 @@
     <t xml:space="preserve">0402_RES</t>
   </si>
   <si>
+    <t xml:space="preserve">R20,R21,R22,R23,R24,R25,R26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 100K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-100KLRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-07100KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPACITOR1210_CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1210_CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C15,C16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 100UF 10V X5R 1210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-9969-6-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM32ER61A107ME20L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9,R10,R11,R12,R13,R14,R15,R16,R17,R18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 10K OHM 1% 1/16W 0402 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-10.0KLRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-0710KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2,C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 10000PF 16V X7R 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-4762-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCM155R71H103KA55D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C13,C14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 10UF 6.3V X5R 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-13211-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRJ155R60J106ME11D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R37,R38,R39,R40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 1M OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-1.00MLRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-071ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERRITE_BEAD0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L2,L3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERRITE BEAD 1 KOHM 0402 1LN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-4003-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLM15HD102SN1D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 1K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-1.00KLRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-071KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10,C11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 1UF 10V X7S 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-13409-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCM155C71A105KE38D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-10448-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM155D71A225ME15D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPOL-USE5-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E5-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLARIZED CAPACITOR, American symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP ALUM 2000UF 20% 6.3V T/H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P122284TB-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EEU-FS0J202B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300VAC - 500ma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MICRO_FUSE500MA_350VAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIRCRO_FUSE_5MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 5mm AC micro fuse package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUSE BRD MNT 500MA 350VAC 100VDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">507-1903-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bel Fuse Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0697H0500-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 34K OHM 1% 1/10W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P34.0KLCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2RKF3402X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 4.7UF 6.3V X5R 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-5408-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM155R60J475ME87D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.99k</t>
+  </si>
+  <si>
     <t xml:space="preserve">R6,R7</t>
   </si>
   <si>
-    <t xml:space="preserve">Resistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 1.5K OHM 0.1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P1.5KDCCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panasonic Electronic Components</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERA-2AEB152X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R21,R22,R23,R24,R25,R26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 100K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">541-100KLCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay Dale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRCW0402100KFKED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAPACITOR1210_CAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1210_CAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C15,C16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 100UF 6.3V X7S 1210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-10530-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM32EC70J107ME15L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R11,R12,R13,R14,R15,R16,R17,R18,R19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 10K OHM 1% 1/16W 0402 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RMCF0402FT10K0CT-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stackpole Electronics Inc. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RMCF0402FT10K0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2,C3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 10000PF 16V X7R 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-1313-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM155R71C103KA01D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C13,C14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 10UF 6.3V X5R 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-13211-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRJ155R60J106ME11D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R37,R38,R39,R40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES 1M OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RMCF0402FT1M00CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stackpole Electronics Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RMCF0402FT1M00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FERRITE_BEAD0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L2,L3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FERRITE BEAD 1 KOHM 0402 1LN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-4003-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Murata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BLM15HD102SN1D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 1K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RMCF0402FT1K00CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stackpole Electronics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RMCF0402FT1K00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C10,C11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 1UF 10V X7S 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-13409-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCM155C71A105KE38D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.2uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-12696-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM155C70J225KE11D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2000uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPOL-USE5-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E5-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POLARIZED CAPACITOR, American symbol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP ALUM 2000UF 20% 6.3V T/H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P122284TB-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEU-FS0J202B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300VAC - 500ma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MICRO_FUSE500MA_350VAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIRCRO_FUSE_5MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A 5mm AC micro fuse package</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUSE BRD MNT 500MA 350VAC 100VDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">507-1903-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bel Fuse Inc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0697H0500-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 34K OHM 1% 1/10W 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P34.0KLCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-2RKF3402X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.7uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 4.7UF 6.3V X5R 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">445-5947-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TDK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1005X5R0J475K050BC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.99k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8,R9</t>
-  </si>
-  <si>
     <t xml:space="preserve">RES SMD 4.99K OHM 1% 1/10W 0402</t>
   </si>
   <si>
@@ -526,7 +484,7 @@
     <t xml:space="preserve">5.1k</t>
   </si>
   <si>
-    <t xml:space="preserve">R10</t>
+    <t xml:space="preserve">R8</t>
   </si>
   <si>
     <t xml:space="preserve">RES SMD 5.1K OHM 1% 1/10W 0402</t>
@@ -577,10 +535,10 @@
     <t xml:space="preserve">RES SMD 68 OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">311-68.0LRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0402FR-0768RL</t>
+    <t xml:space="preserve">P68.0LCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2RKF68R0X</t>
   </si>
   <si>
     <t xml:space="preserve">750k</t>
@@ -712,7 +670,7 @@
     <t xml:space="preserve">LED-0603</t>
   </si>
   <si>
-    <t xml:space="preserve">D9</t>
+    <t xml:space="preserve">D5</t>
   </si>
   <si>
     <t xml:space="preserve">LED</t>
@@ -826,6 +784,9 @@
     <t xml:space="preserve">IRM-03-5</t>
   </si>
   <si>
+    <t xml:space="preserve">LIS2DH12</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIS2DW12</t>
   </si>
   <si>
@@ -838,16 +799,16 @@
     <t xml:space="preserve">ultra low power 3 axis accelerometer</t>
   </si>
   <si>
-    <t xml:space="preserve">497-17718-6-ND</t>
+    <t xml:space="preserve">497-14851-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">STMicroelectronics</t>
   </si>
   <si>
-    <t xml:space="preserve">511-LIS2DW12TR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIS2DW12TR</t>
+    <t xml:space="preserve">511-LIS2DH12TR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIS2DH12TR</t>
   </si>
   <si>
     <t xml:space="preserve">MAX-M8</t>
@@ -880,7 +841,7 @@
     <t xml:space="preserve">A simple watchdog timer with adjustable timeouts and reset time</t>
   </si>
   <si>
-    <t xml:space="preserve">MAX6749KA</t>
+    <t xml:space="preserve">MAX6749KA+TCT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">MAX6749KA+T</t>
@@ -949,13 +910,31 @@
     <t xml:space="preserve">F6QA1G582H2JM-J</t>
   </si>
   <si>
+    <t xml:space="preserve">SCREW_TERMNIAL_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">360272-TERMINAL-BLOCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2,J3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A small, single terminal block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1849-1246-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METZ CONNECT USA Inc.</t>
+  </si>
+  <si>
     <t xml:space="preserve">SIP32510</t>
   </si>
   <si>
     <t xml:space="preserve">TSOT23-6</t>
   </si>
   <si>
-    <t xml:space="preserve">U11,U12,U13</t>
+    <t xml:space="preserve">U11,U12,U13,U14</t>
   </si>
   <si>
     <t xml:space="preserve">Load switch, slew rate controlled. By Vishay</t>
@@ -968,33 +947,6 @@
   </si>
   <si>
     <t xml:space="preserve">SIP32510DT-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST_POINT_0.040IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TESTPOINT_0.040IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP1,TP2,TP3,TP4,TP5,TP6,TP7,TP8,TP9,TP10,TP11,TP12,TP13,TP14,TP15,TP16,TP17,TP18,TP19,TP20,TP21,TP22,TP23,TP24,TP25,TP26,TP27,TP28,TP29,TP30,TP31,TP32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.040in Test Point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5001K-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST_POINT_0.060IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TESTPOINT_0.060IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC/L,AC/N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A 60mil Testpoint</t>
   </si>
   <si>
     <t xml:space="preserve">WRL-13678</t>
@@ -1102,26 +1054,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.21428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="145.469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.3265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.2244897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3214285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.1224489795918"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.47959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="147.877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.4642857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.4387755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.6632653061224"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.1275510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.7959183673469"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -1176,69 +1128,72 @@
       <c r="E2" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="H2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,22 +1201,25 @@
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>33</v>
@@ -1269,89 +1227,95 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="H7" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>48</v>
+        <v>58</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1359,63 +1323,63 @@
         <v>2</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1423,95 +1387,95 @@
         <v>2</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="D11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="F11" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="0" t="s">
+      <c r="H11" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="I11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="F12" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="I12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="H13" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="0" t="s">
+      <c r="I13" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="K13" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1519,28 +1483,25 @@
         <v>2</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="I14" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>56</v>
       </c>
       <c r="K14" s="0" t="s">
         <v>95</v>
@@ -1548,34 +1509,34 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="F15" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="0" t="s">
+      <c r="H15" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="I15" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1583,28 +1544,31 @@
         <v>2</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="H16" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="I16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,62 +1576,62 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="0" t="s">
+      <c r="H18" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="F18" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" s="0" t="s">
+      <c r="I18" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="K18" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="I18" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K18" s="0" t="s">
+      <c r="L18" s="0" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1679,25 +1643,28 @@
         <v>119</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>48</v>
+        <v>123</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>124</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>56</v>
+        <v>126</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,34 +1672,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>124</v>
+        <v>55</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>125</v>
+        <v>56</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="L20" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,63 +1704,63 @@
         <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>133</v>
+        <v>41</v>
       </c>
       <c r="D21" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="F21" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="H21" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="I21" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="K21" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="H22" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="0" t="s">
+      <c r="I22" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="K22" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,63 +1768,63 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="H23" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="0" t="s">
+      <c r="I23" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="K23" s="0" t="s">
         <v>147</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="K24" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,31 +1832,31 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="K25" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="K25" s="0" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1900,284 +1864,278 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="G26" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="0" t="s">
+      <c r="H26" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="F26" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G26" s="0" t="s">
+      <c r="I26" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="K26" s="0" t="s">
         <v>164</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="K26" s="0" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="0" t="n">
+        <v>66.5</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="H27" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="0" t="s">
+      <c r="I27" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="K27" s="0" t="s">
         <v>168</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B28" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="K28" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="K28" s="0" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>66.5</v>
+        <v>4</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>173</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>59</v>
+        <v>174</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>60</v>
+        <v>175</v>
       </c>
       <c r="E29" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="K29" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="K29" s="0" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>68</v>
+        <v>1</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>180</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E30" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="H30" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="F30" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" s="0" t="s">
+      <c r="I30" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="K30" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="H31" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="I31" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="K31" s="0" t="s">
         <v>189</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="K31" s="0" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>59</v>
+        <v>174</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>60</v>
+        <v>175</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>196</v>
+        <v>58</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>59</v>
+        <v>193</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>51</v>
+        <v>198</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>199</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="E34" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="I34" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="F34" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="H34" s="0" t="s">
+      <c r="K34" s="0" t="s">
         <v>205</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="K34" s="0" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2185,28 +2143,28 @@
         <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="D35" s="0" t="s">
+      <c r="E35" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="G35" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="H35" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="H35" s="0" t="s">
+      <c r="I35" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="I35" s="0" t="s">
+      <c r="K35" s="0" t="s">
         <v>212</v>
-      </c>
-      <c r="K35" s="0" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2217,25 +2175,28 @@
         <v>213</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>218</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,28 +2204,31 @@
         <v>1</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E37" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="K37" s="0" t="s">
         <v>222</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="K37" s="0" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2272,7 +2236,7 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>228</v>
@@ -2286,17 +2250,17 @@
       <c r="F38" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="G38" s="0" t="s">
+      <c r="H38" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="H38" s="0" t="s">
+      <c r="I38" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="I38" s="0" t="s">
+      <c r="K38" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="L38" s="0" t="s">
         <v>234</v>
-      </c>
-      <c r="K38" s="0" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2304,10 +2268,10 @@
         <v>1</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>236</v>
@@ -2315,20 +2279,17 @@
       <c r="E39" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="G39" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="G39" s="0" t="s">
+      <c r="H39" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="H39" s="0" t="s">
+      <c r="I39" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="I39" s="0" t="s">
+      <c r="K39" s="0" t="s">
         <v>241</v>
-      </c>
-      <c r="K39" s="0" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2347,20 +2308,17 @@
       <c r="E40" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="F40" s="0" t="s">
+      <c r="G40" s="0" t="s">
         <v>245</v>
       </c>
       <c r="H40" s="0" t="s">
         <v>246</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>247</v>
+        <v>47</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="L40" s="0" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2368,28 +2326,28 @@
         <v>1</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="C41" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="D41" s="0" t="s">
+      <c r="F41" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="H41" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="G41" s="0" t="s">
+      <c r="I41" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="H41" s="0" t="s">
+      <c r="K41" s="0" t="s">
         <v>253</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="K41" s="0" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,28 +2355,31 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="D42" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="D42" s="0" t="s">
+      <c r="E42" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="F42" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="G42" s="0" t="s">
+      <c r="H42" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="H42" s="0" t="s">
+      <c r="I42" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="I42" s="0" t="s">
-        <v>51</v>
+      <c r="J42" s="0" t="s">
+        <v>261</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2426,28 +2387,28 @@
         <v>1</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="F43" s="0" t="s">
         <v>264</v>
       </c>
+      <c r="G43" s="0" t="s">
+        <v>265</v>
+      </c>
       <c r="H43" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2455,42 +2416,39 @@
         <v>1</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="J44" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="K44" s="0" t="s">
         <v>274</v>
-      </c>
-      <c r="K44" s="0" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>276</v>
@@ -2498,17 +2456,14 @@
       <c r="E45" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="G45" s="0" t="s">
+      <c r="H45" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="H45" s="0" t="s">
+      <c r="I45" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="I45" s="0" t="s">
+      <c r="K45" s="0" t="s">
         <v>280</v>
-      </c>
-      <c r="K45" s="0" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2516,25 +2471,28 @@
         <v>1</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="E46" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="D46" s="0" t="s">
+      <c r="F46" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="G46" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="H46" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="H46" s="0" t="s">
+      <c r="I46" s="0" t="s">
         <v>286</v>
-      </c>
-      <c r="I46" s="0" t="s">
-        <v>247</v>
       </c>
       <c r="K46" s="0" t="s">
         <v>287</v>
@@ -2542,68 +2500,68 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>288</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>292</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="K47" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="G48" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="K48" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
+      </c>
+      <c r="K48" s="0" t="n">
+        <v>360272</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>302</v>
@@ -2614,7 +2572,7 @@
       <c r="E49" s="0" t="s">
         <v>304</v>
       </c>
-      <c r="G49" s="0" t="s">
+      <c r="F49" s="0" t="s">
         <v>305</v>
       </c>
       <c r="H49" s="0" t="s">
@@ -2629,7 +2587,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>309</v>
@@ -2638,94 +2596,22 @@
         <v>309</v>
       </c>
       <c r="D50" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="E50" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="E50" s="0" t="s">
+      <c r="F50" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="H50" s="0" t="s">
         <v>312</v>
-      </c>
-      <c r="H50" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="I50" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="K50" s="0" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>317</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="H51" s="0" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>328</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>